<commit_message>
change view model 6 and 12 view
</commit_message>
<xml_diff>
--- a/Document/Task.xlsx
+++ b/Document/Task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Что сделать</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t xml:space="preserve">сущность для страницы что выше </t>
+  </si>
+  <si>
+    <t>может добавить модальное окно</t>
   </si>
 </sst>
 </file>
@@ -496,6 +499,9 @@
       <c r="F7" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="3:9">
       <c r="C8" s="1">

</xml_diff>